<commit_message>
added log4j.properties added test case file updated gitignore updated chromedriver.exe removed unused files
</commit_message>
<xml_diff>
--- a/src/main/resources/TestData.xlsx
+++ b/src/main/resources/TestData.xlsx
@@ -3,20 +3,20 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Project\BioFourmis_Demo\BioFourmisDemoFinal\src\main\resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Project\TestApp\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="15435" windowHeight="7380"/>
   </bookViews>
   <sheets>
-    <sheet name="TestDataSheet" sheetId="1" r:id="rId1"/>
+    <sheet name="BrandingPage" sheetId="2" r:id="rId1"/>
   </sheets>
   <calcPr calcId="0"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -24,102 +24,68 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="26">
-  <si>
-    <t>firstname</t>
-  </si>
-  <si>
-    <t>lastname</t>
-  </si>
-  <si>
-    <t>password</t>
-  </si>
-  <si>
-    <t>city</t>
-  </si>
-  <si>
-    <t>state</t>
-  </si>
-  <si>
-    <t>address</t>
-  </si>
-  <si>
-    <t>Welcome@123</t>
-  </si>
-  <si>
-    <t>Charlotte</t>
-  </si>
-  <si>
-    <t>Michigan</t>
-  </si>
-  <si>
-    <t>postalCode</t>
-  </si>
-  <si>
-    <t>+19197175772</t>
-  </si>
-  <si>
-    <t>48813</t>
-  </si>
-  <si>
-    <t>usernameone</t>
-  </si>
-  <si>
-    <t>TestFirstnameone</t>
-  </si>
-  <si>
-    <t>TestFirstnametwo</t>
-  </si>
-  <si>
-    <t>TestFirstnamethree</t>
-  </si>
-  <si>
-    <t>TestFirstnamefour</t>
-  </si>
-  <si>
-    <t>TestFirstnameFive</t>
-  </si>
-  <si>
-    <t>usernameTwo</t>
-  </si>
-  <si>
-    <t>usernameThree</t>
-  </si>
-  <si>
-    <t>usernameFour</t>
-  </si>
-  <si>
-    <t>usernameFive</t>
-  </si>
-  <si>
-    <t>testmail</t>
-  </si>
-  <si>
-    <t>emailAddress</t>
-  </si>
-  <si>
-    <t>Changi Business Park</t>
-  </si>
-  <si>
-    <t>mobilePhone</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="17">
+  <si>
+    <t>MainHeader1</t>
+  </si>
+  <si>
+    <t>MainHeader2</t>
+  </si>
+  <si>
+    <t>Subtext</t>
+  </si>
+  <si>
+    <t>Healthcare Branding Services: Be Professional, Recognizable and Different</t>
+  </si>
+  <si>
+    <t>Your brand is who you are. Be your best.</t>
+  </si>
+  <si>
+    <t>Developing and communicating how and why you’re different.</t>
+  </si>
+  <si>
+    <t>Experienced professionals who have created thousands of brands.</t>
+  </si>
+  <si>
+    <t>Most doctors and executives now recognize that healthcare branding is vital. At the same time, branding is often misunderstood. Your brand is not merely your logo or even your brand identity package. Rather, your brand is the much larger sum of every experience the patient has with your hospital, practice or healthcare organization. That includes everything from signage, the voice on the phone, to the quality of customer care and patient experience. Everything.</t>
+  </si>
+  <si>
+    <t>It’s your organization’s personality, presence, reputation, vision, mission, capabilities, philosophy and style. In turn, patients form their impression of your organization based upon all these things. At Healthcare Success, we help you take charge of that perception… and then mold it into a compelling and unique brand.</t>
+  </si>
+  <si>
+    <t>Our branding services are an essential part of success. How you communicate your branding message is at the very heart of marketing. In fact, marketing is the active, informed, strategic and measured communication of what makes you unique and important to those whom you most want to reach. Your message of unique value is expressed in your logo, brochure, videos and throughout all the elements of your plan.</t>
+  </si>
+  <si>
+    <t>So who are these people or organizations? How do you get their attention and address their needs? What best drives their response? What do they need to hear? To see? To understand? How should you present your brand for maximum appeal, understanding and persuasiveness?</t>
+  </si>
+  <si>
+    <t>The answers are not the same for everyone. Of course, that’s where we come in.</t>
+  </si>
+  <si>
+    <t>Healthcare Success delivers full-service branding that ensures that every aspect of your message will engage the audience and drive response. Our marketing professionals have years of successful experience creating effective branding tools, such as logos with distinction, brochures that differentiate, and compelling videos. Throughout your plan, we create distinction that is memorable and exclusive.</t>
+  </si>
+  <si>
+    <t>For more information about our branding services, call us today at 866-639-5049. We’ll create a compelling, professional and well-differentiated brand that sets you above the rest.</t>
+  </si>
+  <si>
+    <t>For more information about our branding services, call us today at 866-938-8016. We’ll create a compelling, professional and well-differentiated brand that sets you above the rest.</t>
+  </si>
+  <si>
+    <t>For more information about our branding services, call us today at 800-656-0907. We’ll create a compelling, professional and well-differentiated brand that sets you above the rest.</t>
+  </si>
+  <si>
+    <t>For more information about our branding services, call us today at 866-348-1742. We’ll create a compelling, professional and well-differentiated brand that sets you above the rest.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <numFmts count="0"/>
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -142,17 +108,16 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -465,203 +430,81 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I6"/>
+  <dimension ref="A1:C8"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="38" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="21.140625" customWidth="1"/>
-    <col min="3" max="4" width="17.28515625" customWidth="1"/>
-    <col min="5" max="5" width="19.42578125" customWidth="1"/>
-    <col min="6" max="6" width="12.42578125" customWidth="1"/>
-    <col min="8" max="8" width="11" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" style="1" width="67.09375" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" style="1" width="60.16015625" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" style="1" width="255.0" collapsed="true"/>
+    <col min="4" max="4" style="1" width="38.0" collapsed="true"/>
+    <col min="5" max="16384" style="1" width="38.0" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>23</v>
-      </c>
-      <c r="B1" t="s">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D1" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" t="s">
+    </row>
+    <row r="2" spans="1:3" ht="180" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="135" x14ac:dyDescent="0.25">
+      <c r="B3" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="F1" t="s">
-        <v>3</v>
-      </c>
-      <c r="G1" t="s">
-        <v>4</v>
-      </c>
-      <c r="H1" t="s">
+      <c r="C3" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="180" x14ac:dyDescent="0.25">
+      <c r="B4" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="I1" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>22</v>
-      </c>
-      <c r="B2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C2" t="s">
+    </row>
+    <row r="5" spans="1:3" ht="120" x14ac:dyDescent="0.25">
+      <c r="C5" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="C6" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="165" x14ac:dyDescent="0.25">
+      <c r="C7" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="D2" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="E2" t="s">
-        <v>24</v>
-      </c>
-      <c r="F2" t="s">
-        <v>7</v>
-      </c>
-      <c r="G2" t="s">
-        <v>8</v>
-      </c>
-      <c r="H2" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="I2" s="2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>22</v>
-      </c>
-      <c r="B3" t="s">
+    </row>
+    <row r="8" spans="1:3" ht="75" x14ac:dyDescent="0.25">
+      <c r="C8" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C3" t="s">
-        <v>18</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="E3" t="s">
-        <v>24</v>
-      </c>
-      <c r="F3" t="s">
-        <v>7</v>
-      </c>
-      <c r="G3" t="s">
-        <v>8</v>
-      </c>
-      <c r="H3" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="I3" s="2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>22</v>
-      </c>
-      <c r="B4" t="s">
-        <v>15</v>
-      </c>
-      <c r="C4" t="s">
-        <v>19</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="E4" t="s">
-        <v>24</v>
-      </c>
-      <c r="F4" t="s">
-        <v>7</v>
-      </c>
-      <c r="G4" t="s">
-        <v>8</v>
-      </c>
-      <c r="H4" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="I4" s="2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>22</v>
-      </c>
-      <c r="B5" t="s">
-        <v>16</v>
-      </c>
-      <c r="C5" t="s">
-        <v>20</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="E5" t="s">
-        <v>24</v>
-      </c>
-      <c r="F5" t="s">
-        <v>7</v>
-      </c>
-      <c r="G5" t="s">
-        <v>8</v>
-      </c>
-      <c r="H5" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="I5" s="2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>22</v>
-      </c>
-      <c r="B6" t="s">
-        <v>17</v>
-      </c>
-      <c r="C6" t="s">
-        <v>21</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="E6" t="s">
-        <v>24</v>
-      </c>
-      <c r="F6" t="s">
-        <v>7</v>
-      </c>
-      <c r="G6" t="s">
-        <v>8</v>
-      </c>
-      <c r="H6" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="I6" s="2" t="s">
-        <v>10</v>
-      </c>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="D2" r:id="rId1"/>
-    <hyperlink ref="D3:D6" r:id="rId2" display="Welcome@123"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>